<commit_message>
Updated table with a few more comments.
</commit_message>
<xml_diff>
--- a/questions/Assignment5-BLEEventSchedulerGuidance.xlsx
+++ b/questions/Assignment5-BLEEventSchedulerGuidance.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>A5 Command Table</t>
   </si>
@@ -75,7 +75,7 @@
     <t>sl_bt_advertiser_create_set()</t>
   </si>
   <si>
-    <t>Creates an advertising set to use when the slave device wants to advertise its presence</t>
+    <t>Creates an advertising set to use when the slave device wants to advertise its presence. The handle created by this call is only to be used for advertising API calls.</t>
   </si>
   <si>
     <t>sl_bt_advertiser_set_timing()</t>
@@ -105,7 +105,7 @@
     <t>Stop advertising</t>
   </si>
   <si>
-    <t>Save this connection handle. Use this value in all subsequent calls when this connection is open to the client.</t>
+    <t>Save this connection handle. Use this value in all subsequent calls that require a connect handle, when this connection is open to the client.</t>
   </si>
   <si>
     <t>sl_bt_connection_set_parameters()</t>
@@ -150,7 +150,62 @@
     </r>
   </si>
   <si>
-    <t>Please note: Every semester students fail to check first for the event ID = sl_bt_evt_system_external_signal_id and then check for the event value in evt-&gt;data.evt_system_external_signal.extsignals</t>
+    <t>For this assignment these are our events from LETIMER0 and the I2C transfers.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Please note: Every semester students fail to check first for the event ID = sl_bt_evt_system_external_signal_id and then check for the event value in evt-&gt;data.evt_system_external_signal.extsignals.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Your state machine should call sl_bt_gatt_server_send_indication() if the appropriate conditions are met:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Connection is open
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Client has enabled indications for the HTM indications
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>There is no indication currently in-flight</t>
+    </r>
   </si>
   <si>
     <t>Events only for Slaves/Servers</t>
@@ -189,6 +244,9 @@
   <si>
     <t>Track whether indications are enabled/disabled for each and every characteristic. Indications for each characteristic value is independently controllable from the client.
 Track whether an indication is in flight or not.</t>
+  </si>
+  <si>
+    <t>Structure your case statement here to handle both of these cases.</t>
   </si>
   <si>
     <t>sl_bt_evt_gatt_server_indication_timeout_id</t>
@@ -1491,7 +1549,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" ht="26.1" customHeight="1">
+    <row r="5" ht="39.1" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1632,7 +1690,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" ht="64.9" customHeight="1">
+    <row r="16" ht="168.9" customHeight="1">
       <c r="A16" s="8"/>
       <c r="B16" t="s" s="6">
         <v>31</v>
@@ -1642,9 +1700,11 @@
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="F16" t="s" s="11">
+        <v>33</v>
+      </c>
       <c r="G16" t="s" s="12">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" ht="13.1" customHeight="1">
@@ -1658,7 +1718,7 @@
     </row>
     <row r="18" ht="14.35" customHeight="1">
       <c r="A18" t="s" s="6">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -1670,17 +1730,19 @@
     <row r="19" ht="110.35" customHeight="1">
       <c r="A19" s="8"/>
       <c r="B19" t="s" s="6">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s" s="13">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s" s="11">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
-      <c r="G19" s="10"/>
+      <c r="G19" t="s" s="12">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" ht="13.1" customHeight="1">
       <c r="A20" s="8"/>
@@ -1694,13 +1756,13 @@
     <row r="21" ht="50.35" customHeight="1">
       <c r="A21" s="8"/>
       <c r="B21" t="s" s="6">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s" s="13">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s" s="11">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>

</xml_diff>